<commit_message>
regenerated Sympheny input files
</commit_message>
<xml_diff>
--- a/PythonResources/Data/Consumption/Sympheny/base_1045_coo.xlsx
+++ b/PythonResources/Data/Consumption/Sympheny/base_1045_coo.xlsx
@@ -23679,7 +23679,7 @@
         <v>2917</v>
       </c>
       <c r="B2917">
-        <v>3.712711839073521</v>
+        <v>3.71271183907352</v>
       </c>
     </row>
     <row r="2918" spans="1:2">
@@ -23703,7 +23703,7 @@
         <v>2920</v>
       </c>
       <c r="B2920">
-        <v>5.357367893833258</v>
+        <v>5.357367893833257</v>
       </c>
     </row>
     <row r="2921" spans="1:2">
@@ -24847,7 +24847,7 @@
         <v>3063</v>
       </c>
       <c r="B3063">
-        <v>7.958138905121769</v>
+        <v>7.958138905121768</v>
       </c>
     </row>
     <row r="3064" spans="1:2">
@@ -24855,7 +24855,7 @@
         <v>3064</v>
       </c>
       <c r="B3064">
-        <v>1.847475867065322</v>
+        <v>1.847475867065321</v>
       </c>
     </row>
     <row r="3065" spans="1:2">
@@ -25431,7 +25431,7 @@
         <v>3136</v>
       </c>
       <c r="B3136">
-        <v>8.723464615482007</v>
+        <v>8.723464615482005</v>
       </c>
     </row>
     <row r="3137" spans="1:2">
@@ -26399,7 +26399,7 @@
         <v>3257</v>
       </c>
       <c r="B3257">
-        <v>7.813215276503733</v>
+        <v>7.813215276503732</v>
       </c>
     </row>
     <row r="3258" spans="1:2">
@@ -26535,7 +26535,7 @@
         <v>3274</v>
       </c>
       <c r="B3274">
-        <v>7.208433881122182</v>
+        <v>7.208433881122181</v>
       </c>
     </row>
     <row r="3275" spans="1:2">
@@ -26543,7 +26543,7 @@
         <v>3275</v>
       </c>
       <c r="B3275">
-        <v>9.95456812758672</v>
+        <v>9.954568127586718</v>
       </c>
     </row>
     <row r="3276" spans="1:2">
@@ -28143,7 +28143,7 @@
         <v>3475</v>
       </c>
       <c r="B3475">
-        <v>2.626159755367743</v>
+        <v>2.626159755367742</v>
       </c>
     </row>
     <row r="3476" spans="1:2">
@@ -28519,7 +28519,7 @@
         <v>3522</v>
       </c>
       <c r="B3522">
-        <v>0.6327022732348185</v>
+        <v>0.6327022732348184</v>
       </c>
     </row>
     <row r="3523" spans="1:2">
@@ -28911,7 +28911,7 @@
         <v>3571</v>
       </c>
       <c r="B3571">
-        <v>6.546884625551927</v>
+        <v>6.546884625551926</v>
       </c>
     </row>
     <row r="3572" spans="1:2">
@@ -29327,7 +29327,7 @@
         <v>3623</v>
       </c>
       <c r="B3623">
-        <v>5.998372869593353</v>
+        <v>5.998372869593352</v>
       </c>
     </row>
     <row r="3624" spans="1:2">
@@ -29455,7 +29455,7 @@
         <v>3639</v>
       </c>
       <c r="B3639">
-        <v>28.41581622335765</v>
+        <v>28.41581622335764</v>
       </c>
     </row>
     <row r="3640" spans="1:2">
@@ -29495,7 +29495,7 @@
         <v>3644</v>
       </c>
       <c r="B3644">
-        <v>9.987890304682514</v>
+        <v>9.987890304682512</v>
       </c>
     </row>
     <row r="3645" spans="1:2">
@@ -30239,7 +30239,7 @@
         <v>3737</v>
       </c>
       <c r="B3737">
-        <v>7.549597877227853</v>
+        <v>7.549597877227852</v>
       </c>
     </row>
     <row r="3738" spans="1:2">
@@ -30247,7 +30247,7 @@
         <v>3738</v>
       </c>
       <c r="B3738">
-        <v>6.462011252755601</v>
+        <v>6.4620112527556</v>
       </c>
     </row>
     <row r="3739" spans="1:2">
@@ -30263,7 +30263,7 @@
         <v>3740</v>
       </c>
       <c r="B3740">
-        <v>0.552816969516509</v>
+        <v>0.5528169695165089</v>
       </c>
     </row>
     <row r="3741" spans="1:2">
@@ -30751,7 +30751,7 @@
         <v>3801</v>
       </c>
       <c r="B3801">
-        <v>14.91382832250241</v>
+        <v>14.9138283225024</v>
       </c>
     </row>
     <row r="3802" spans="1:2">
@@ -30783,7 +30783,7 @@
         <v>3805</v>
       </c>
       <c r="B3805">
-        <v>21.55431983780277</v>
+        <v>21.55431983780276</v>
       </c>
     </row>
     <row r="3806" spans="1:2">
@@ -30791,7 +30791,7 @@
         <v>3806</v>
       </c>
       <c r="B3806">
-        <v>27.50896650842785</v>
+        <v>27.50896650842784</v>
       </c>
     </row>
     <row r="3807" spans="1:2">
@@ -31367,7 +31367,7 @@
         <v>3878</v>
       </c>
       <c r="B3878">
-        <v>7.061986283103107</v>
+        <v>7.061986283103106</v>
       </c>
     </row>
     <row r="3879" spans="1:2">
@@ -31527,7 +31527,7 @@
         <v>3898</v>
       </c>
       <c r="B3898">
-        <v>12.24626642150298</v>
+        <v>12.24626642150297</v>
       </c>
     </row>
     <row r="3899" spans="1:2">
@@ -31567,7 +31567,7 @@
         <v>3903</v>
       </c>
       <c r="B3903">
-        <v>20.53765640468656</v>
+        <v>20.53765640468655</v>
       </c>
     </row>
     <row r="3904" spans="1:2">
@@ -31783,7 +31783,7 @@
         <v>3930</v>
       </c>
       <c r="B3930">
-        <v>21.42255509882063</v>
+        <v>21.42255509882062</v>
       </c>
     </row>
     <row r="3931" spans="1:2">
@@ -31847,7 +31847,7 @@
         <v>3938</v>
       </c>
       <c r="B3938">
-        <v>5.190346708900158</v>
+        <v>5.190346708900157</v>
       </c>
     </row>
     <row r="3939" spans="1:2">
@@ -31863,7 +31863,7 @@
         <v>3940</v>
       </c>
       <c r="B3940">
-        <v>3.715994234706528</v>
+        <v>3.715994234706527</v>
       </c>
     </row>
     <row r="3941" spans="1:2">
@@ -31959,7 +31959,7 @@
         <v>3952</v>
       </c>
       <c r="B3952">
-        <v>32.145203804531</v>
+        <v>32.14520380453099</v>
       </c>
     </row>
     <row r="3953" spans="1:2">
@@ -31975,7 +31975,7 @@
         <v>3954</v>
       </c>
       <c r="B3954">
-        <v>28.45447229335708</v>
+        <v>28.45447229335707</v>
       </c>
     </row>
     <row r="3955" spans="1:2">
@@ -32055,7 +32055,7 @@
         <v>3964</v>
       </c>
       <c r="B3964">
-        <v>7.49602449136056</v>
+        <v>7.496024491360559</v>
       </c>
     </row>
     <row r="3965" spans="1:2">
@@ -32087,7 +32087,7 @@
         <v>3968</v>
       </c>
       <c r="B3968">
-        <v>21.32727770415183</v>
+        <v>21.32727770415182</v>
       </c>
     </row>
     <row r="3969" spans="1:2">
@@ -32255,7 +32255,7 @@
         <v>3989</v>
       </c>
       <c r="B3989">
-        <v>6.135500808582997</v>
+        <v>6.135500808582996</v>
       </c>
     </row>
     <row r="3990" spans="1:2">
@@ -32263,7 +32263,7 @@
         <v>3990</v>
       </c>
       <c r="B3990">
-        <v>6.864251253318297</v>
+        <v>6.864251253318296</v>
       </c>
     </row>
     <row r="3991" spans="1:2">
@@ -32687,7 +32687,7 @@
         <v>4043</v>
       </c>
       <c r="B4043">
-        <v>22.7955343007413</v>
+        <v>22.79553430074129</v>
       </c>
     </row>
     <row r="4044" spans="1:2">
@@ -32695,7 +32695,7 @@
         <v>4044</v>
       </c>
       <c r="B4044">
-        <v>25.87500754657925</v>
+        <v>25.87500754657924</v>
       </c>
     </row>
     <row r="4045" spans="1:2">
@@ -32719,7 +32719,7 @@
         <v>4047</v>
       </c>
       <c r="B4047">
-        <v>35.64066208264487</v>
+        <v>35.64066208264486</v>
       </c>
     </row>
     <row r="4048" spans="1:2">
@@ -32759,7 +32759,7 @@
         <v>4052</v>
       </c>
       <c r="B4052">
-        <v>15.26917695687929</v>
+        <v>15.26917695687928</v>
       </c>
     </row>
     <row r="4053" spans="1:2">
@@ -32863,7 +32863,7 @@
         <v>4065</v>
       </c>
       <c r="B4065">
-        <v>24.2515698350186</v>
+        <v>24.25156983501859</v>
       </c>
     </row>
     <row r="4066" spans="1:2">
@@ -32895,7 +32895,7 @@
         <v>4069</v>
       </c>
       <c r="B4069">
-        <v>31.33046631705246</v>
+        <v>31.33046631705245</v>
       </c>
     </row>
     <row r="4070" spans="1:2">
@@ -32975,7 +32975,7 @@
         <v>4079</v>
       </c>
       <c r="B4079">
-        <v>9.240090242434226</v>
+        <v>9.240090242434224</v>
       </c>
     </row>
     <row r="4080" spans="1:2">
@@ -33007,7 +33007,7 @@
         <v>4083</v>
       </c>
       <c r="B4083">
-        <v>5.838971531665448</v>
+        <v>5.838971531665447</v>
       </c>
     </row>
     <row r="4084" spans="1:2">
@@ -33087,7 +33087,7 @@
         <v>4093</v>
       </c>
       <c r="B4093">
-        <v>31.10128476481929</v>
+        <v>31.10128476481928</v>
       </c>
     </row>
     <row r="4094" spans="1:2">
@@ -33175,7 +33175,7 @@
         <v>4104</v>
       </c>
       <c r="B4104">
-        <v>3.847934816311866</v>
+        <v>3.847934816311865</v>
       </c>
     </row>
     <row r="4105" spans="1:2">
@@ -33191,7 +33191,7 @@
         <v>4106</v>
       </c>
       <c r="B4106">
-        <v>3.517673062844396</v>
+        <v>3.517673062844395</v>
       </c>
     </row>
     <row r="4107" spans="1:2">
@@ -33247,7 +33247,7 @@
         <v>4113</v>
       </c>
       <c r="B4113">
-        <v>20.59178662552732</v>
+        <v>20.59178662552731</v>
       </c>
     </row>
     <row r="4114" spans="1:2">
@@ -33255,7 +33255,7 @@
         <v>4114</v>
       </c>
       <c r="B4114">
-        <v>22.40012285537941</v>
+        <v>22.4001228553794</v>
       </c>
     </row>
     <row r="4115" spans="1:2">
@@ -33279,7 +33279,7 @@
         <v>4117</v>
       </c>
       <c r="B4117">
-        <v>31.89873106101681</v>
+        <v>31.8987310610168</v>
       </c>
     </row>
     <row r="4118" spans="1:2">
@@ -33343,7 +33343,7 @@
         <v>4125</v>
       </c>
       <c r="B4125">
-        <v>8.094915158865019</v>
+        <v>8.094915158865017</v>
       </c>
     </row>
     <row r="4126" spans="1:2">
@@ -33431,7 +33431,7 @@
         <v>4136</v>
       </c>
       <c r="B4136">
-        <v>17.88770807311068</v>
+        <v>17.88770807311067</v>
       </c>
     </row>
     <row r="4137" spans="1:2">
@@ -33471,7 +33471,7 @@
         <v>4141</v>
       </c>
       <c r="B4141">
-        <v>26.7002955914496</v>
+        <v>26.70029559144959</v>
       </c>
     </row>
     <row r="4142" spans="1:2">
@@ -33479,7 +33479,7 @@
         <v>4142</v>
       </c>
       <c r="B4142">
-        <v>27.50175696087678</v>
+        <v>27.50175696087677</v>
       </c>
     </row>
     <row r="4143" spans="1:2">
@@ -33623,7 +33623,7 @@
         <v>4160</v>
       </c>
       <c r="B4160">
-        <v>6.259118172690352</v>
+        <v>6.259118172690351</v>
       </c>
     </row>
     <row r="4161" spans="1:2">
@@ -33911,7 +33911,7 @@
         <v>4196</v>
       </c>
       <c r="B4196">
-        <v>8.639997983671256</v>
+        <v>8.639997983671254</v>
       </c>
     </row>
     <row r="4197" spans="1:2">
@@ -33935,7 +33935,7 @@
         <v>4199</v>
       </c>
       <c r="B4199">
-        <v>7.557774559206505</v>
+        <v>7.557774559206504</v>
       </c>
     </row>
     <row r="4200" spans="1:2">
@@ -33943,7 +33943,7 @@
         <v>4200</v>
       </c>
       <c r="B4200">
-        <v>7.25309790741417</v>
+        <v>7.253097907414169</v>
       </c>
     </row>
     <row r="4201" spans="1:2">
@@ -34047,7 +34047,7 @@
         <v>4213</v>
       </c>
       <c r="B4213">
-        <v>25.47074535584979</v>
+        <v>25.47074535584978</v>
       </c>
     </row>
     <row r="4214" spans="1:2">
@@ -34191,7 +34191,7 @@
         <v>4231</v>
       </c>
       <c r="B4231">
-        <v>8.890280650688045</v>
+        <v>8.890280650688043</v>
       </c>
     </row>
     <row r="4232" spans="1:2">
@@ -34471,7 +34471,7 @@
         <v>4266</v>
       </c>
       <c r="B4266">
-        <v>11.59937071786579</v>
+        <v>11.59937071786578</v>
       </c>
     </row>
     <row r="4267" spans="1:2">
@@ -34479,7 +34479,7 @@
         <v>4267</v>
       </c>
       <c r="B4267">
-        <v>8.789229756557612</v>
+        <v>8.78922975655761</v>
       </c>
     </row>
     <row r="4268" spans="1:2">
@@ -34495,7 +34495,7 @@
         <v>4269</v>
       </c>
       <c r="B4269">
-        <v>4.504091564770752</v>
+        <v>4.504091564770751</v>
       </c>
     </row>
     <row r="4270" spans="1:2">
@@ -34671,7 +34671,7 @@
         <v>4291</v>
       </c>
       <c r="B4291">
-        <v>12.84993414693762</v>
+        <v>12.84993414693761</v>
       </c>
     </row>
     <row r="4292" spans="1:2">
@@ -35247,7 +35247,7 @@
         <v>4363</v>
       </c>
       <c r="B4363">
-        <v>6.882040665365041</v>
+        <v>6.88204066536504</v>
       </c>
     </row>
     <row r="4364" spans="1:2">
@@ -35327,7 +35327,7 @@
         <v>4373</v>
       </c>
       <c r="B4373">
-        <v>3.778945893810985</v>
+        <v>3.778945893810984</v>
       </c>
     </row>
     <row r="4374" spans="1:2">
@@ -35367,7 +35367,7 @@
         <v>4378</v>
       </c>
       <c r="B4378">
-        <v>23.7464325927819</v>
+        <v>23.74643259278189</v>
       </c>
     </row>
     <row r="4379" spans="1:2">
@@ -35375,7 +35375,7 @@
         <v>4379</v>
       </c>
       <c r="B4379">
-        <v>25.33473108680706</v>
+        <v>25.33473108680705</v>
       </c>
     </row>
     <row r="4380" spans="1:2">
@@ -35943,7 +35943,7 @@
         <v>4450</v>
       </c>
       <c r="B4450">
-        <v>18.84716403948019</v>
+        <v>18.84716403948018</v>
       </c>
     </row>
     <row r="4451" spans="1:2">
@@ -35975,7 +35975,7 @@
         <v>4454</v>
       </c>
       <c r="B4454">
-        <v>28.62691529250542</v>
+        <v>28.62691529250541</v>
       </c>
     </row>
     <row r="4455" spans="1:2">
@@ -36271,7 +36271,7 @@
         <v>4491</v>
       </c>
       <c r="B4491">
-        <v>7.057238532276793</v>
+        <v>7.057238532276792</v>
       </c>
     </row>
     <row r="4492" spans="1:2">
@@ -36303,7 +36303,7 @@
         <v>4495</v>
       </c>
       <c r="B4495">
-        <v>8.207688894541905</v>
+        <v>8.207688894541903</v>
       </c>
     </row>
     <row r="4496" spans="1:2">
@@ -36407,7 +36407,7 @@
         <v>4508</v>
       </c>
       <c r="B4508">
-        <v>13.17122792662205</v>
+        <v>13.17122792662204</v>
       </c>
     </row>
     <row r="4509" spans="1:2">
@@ -36455,7 +36455,7 @@
         <v>4514</v>
       </c>
       <c r="B4514">
-        <v>7.222823669120453</v>
+        <v>7.222823669120452</v>
       </c>
     </row>
     <row r="4515" spans="1:2">
@@ -36503,7 +36503,7 @@
         <v>4520</v>
       </c>
       <c r="B4520">
-        <v>7.999725685507814</v>
+        <v>7.999725685507813</v>
       </c>
     </row>
     <row r="4521" spans="1:2">
@@ -36535,7 +36535,7 @@
         <v>4524</v>
       </c>
       <c r="B4524">
-        <v>17.90045666329245</v>
+        <v>17.90045666329244</v>
       </c>
     </row>
     <row r="4525" spans="1:2">
@@ -36831,7 +36831,7 @@
         <v>4561</v>
       </c>
       <c r="B4561">
-        <v>4.792620002332846</v>
+        <v>4.792620002332845</v>
       </c>
     </row>
     <row r="4562" spans="1:2">
@@ -36855,7 +36855,7 @@
         <v>4564</v>
       </c>
       <c r="B4564">
-        <v>3.421604376371207</v>
+        <v>3.421604376371206</v>
       </c>
     </row>
     <row r="4565" spans="1:2">
@@ -37079,7 +37079,7 @@
         <v>4592</v>
       </c>
       <c r="B4592">
-        <v>15.24098352296007</v>
+        <v>15.24098352296006</v>
       </c>
     </row>
     <row r="4593" spans="1:2">
@@ -37271,7 +37271,7 @@
         <v>4616</v>
       </c>
       <c r="B4616">
-        <v>23.06940918637033</v>
+        <v>23.06940918637032</v>
       </c>
     </row>
     <row r="4617" spans="1:2">
@@ -37295,7 +37295,7 @@
         <v>4619</v>
       </c>
       <c r="B4619">
-        <v>25.39349183005866</v>
+        <v>25.39349183005865</v>
       </c>
     </row>
     <row r="4620" spans="1:2">
@@ -37383,7 +37383,7 @@
         <v>4630</v>
       </c>
       <c r="B4630">
-        <v>7.779512107057679</v>
+        <v>7.779512107057678</v>
       </c>
     </row>
     <row r="4631" spans="1:2">
@@ -37391,7 +37391,7 @@
         <v>4631</v>
       </c>
       <c r="B4631">
-        <v>7.525917737304017</v>
+        <v>7.525917737304016</v>
       </c>
     </row>
     <row r="4632" spans="1:2">
@@ -37415,7 +37415,7 @@
         <v>4634</v>
       </c>
       <c r="B4634">
-        <v>6.486365456068359</v>
+        <v>6.486365456068358</v>
       </c>
     </row>
     <row r="4635" spans="1:2">
@@ -37583,7 +37583,7 @@
         <v>4655</v>
       </c>
       <c r="B4655">
-        <v>8.941275011415119</v>
+        <v>8.941275011415117</v>
       </c>
     </row>
     <row r="4656" spans="1:2">
@@ -37623,7 +37623,7 @@
         <v>4660</v>
       </c>
       <c r="B4660">
-        <v>4.30758743334832</v>
+        <v>4.307587433348319</v>
       </c>
     </row>
     <row r="4661" spans="1:2">
@@ -37631,7 +37631,7 @@
         <v>4661</v>
       </c>
       <c r="B4661">
-        <v>3.849400171505173</v>
+        <v>3.849400171505172</v>
       </c>
     </row>
     <row r="4662" spans="1:2">
@@ -38023,7 +38023,7 @@
         <v>4710</v>
       </c>
       <c r="B4710">
-        <v>1.951369550270769</v>
+        <v>1.951369550270768</v>
       </c>
     </row>
     <row r="4711" spans="1:2">
@@ -38055,7 +38055,7 @@
         <v>4714</v>
       </c>
       <c r="B4714">
-        <v>20.6733189884829</v>
+        <v>20.67331898848289</v>
       </c>
     </row>
     <row r="4715" spans="1:2">
@@ -38159,7 +38159,7 @@
         <v>4727</v>
       </c>
       <c r="B4727">
-        <v>8.10643285068441</v>
+        <v>8.106432850684408</v>
       </c>
     </row>
     <row r="4728" spans="1:2">
@@ -38231,7 +38231,7 @@
         <v>4736</v>
       </c>
       <c r="B4736">
-        <v>20.17386732439624</v>
+        <v>20.17386732439623</v>
       </c>
     </row>
     <row r="4737" spans="1:2">
@@ -38383,7 +38383,7 @@
         <v>4755</v>
       </c>
       <c r="B4755">
-        <v>8.716430910554134</v>
+        <v>8.716430910554132</v>
       </c>
     </row>
     <row r="4756" spans="1:2">
@@ -38487,7 +38487,7 @@
         <v>4768</v>
       </c>
       <c r="B4768">
-        <v>31.4605898582181</v>
+        <v>31.46058985821809</v>
       </c>
     </row>
     <row r="4769" spans="1:2">
@@ -38527,7 +38527,7 @@
         <v>4773</v>
       </c>
       <c r="B4773">
-        <v>17.75661739751746</v>
+        <v>17.75661739751745</v>
       </c>
     </row>
     <row r="4774" spans="1:2">
@@ -38695,7 +38695,7 @@
         <v>4794</v>
       </c>
       <c r="B4794">
-        <v>24.76634911442725</v>
+        <v>24.76634911442724</v>
       </c>
     </row>
     <row r="4795" spans="1:2">
@@ -38807,7 +38807,7 @@
         <v>4808</v>
       </c>
       <c r="B4808">
-        <v>29.06186202098272</v>
+        <v>29.06186202098271</v>
       </c>
     </row>
     <row r="4809" spans="1:2">
@@ -38815,7 +38815,7 @@
         <v>4809</v>
       </c>
       <c r="B4809">
-        <v>32.04321508307685</v>
+        <v>32.04321508307684</v>
       </c>
     </row>
     <row r="4810" spans="1:2">
@@ -38847,7 +38847,7 @@
         <v>4813</v>
       </c>
       <c r="B4813">
-        <v>41.50530663729705</v>
+        <v>41.50530663729704</v>
       </c>
     </row>
     <row r="4814" spans="1:2">
@@ -38871,7 +38871,7 @@
         <v>4816</v>
       </c>
       <c r="B4816">
-        <v>35.0035256445951</v>
+        <v>35.00352564459509</v>
       </c>
     </row>
     <row r="4817" spans="1:2">
@@ -39023,7 +39023,7 @@
         <v>4835</v>
       </c>
       <c r="B4835">
-        <v>18.127147111697</v>
+        <v>18.12714711169699</v>
       </c>
     </row>
     <row r="4836" spans="1:2">
@@ -39167,7 +39167,7 @@
         <v>4853</v>
       </c>
       <c r="B4853">
-        <v>8.486516680724309</v>
+        <v>8.486516680724307</v>
       </c>
     </row>
     <row r="4854" spans="1:2">
@@ -39175,7 +39175,7 @@
         <v>4854</v>
       </c>
       <c r="B4854">
-        <v>9.793584206050042</v>
+        <v>9.79358420605004</v>
       </c>
     </row>
     <row r="4855" spans="1:2">
@@ -39239,7 +39239,7 @@
         <v>4862</v>
       </c>
       <c r="B4862">
-        <v>20.19839737033219</v>
+        <v>20.19839737033218</v>
       </c>
     </row>
     <row r="4863" spans="1:2">
@@ -39351,7 +39351,7 @@
         <v>4876</v>
       </c>
       <c r="B4876">
-        <v>8.585398849168646</v>
+        <v>8.585398849168644</v>
       </c>
     </row>
     <row r="4877" spans="1:2">
@@ -39455,7 +39455,7 @@
         <v>4889</v>
       </c>
       <c r="B4889">
-        <v>35.4569065414042</v>
+        <v>35.45690654140419</v>
       </c>
     </row>
     <row r="4890" spans="1:2">
@@ -39871,7 +39871,7 @@
         <v>4941</v>
       </c>
       <c r="B4941">
-        <v>13.7486657940965</v>
+        <v>13.74866579409649</v>
       </c>
     </row>
     <row r="4942" spans="1:2">
@@ -39887,7 +39887,7 @@
         <v>4943</v>
       </c>
       <c r="B4943">
-        <v>11.32394255573186</v>
+        <v>11.32394255573185</v>
       </c>
     </row>
     <row r="4944" spans="1:2">
@@ -40079,7 +40079,7 @@
         <v>4967</v>
       </c>
       <c r="B4967">
-        <v>8.385934700255735</v>
+        <v>8.385934700255733</v>
       </c>
     </row>
     <row r="4968" spans="1:2">
@@ -40127,7 +40127,7 @@
         <v>4973</v>
       </c>
       <c r="B4973">
-        <v>4.879456951088203</v>
+        <v>4.879456951088202</v>
       </c>
     </row>
     <row r="4974" spans="1:2">
@@ -40151,7 +40151,7 @@
         <v>4976</v>
       </c>
       <c r="B4976">
-        <v>15.48177068832423</v>
+        <v>15.48177068832422</v>
       </c>
     </row>
     <row r="4977" spans="1:2">
@@ -40207,7 +40207,7 @@
         <v>4983</v>
       </c>
       <c r="B4983">
-        <v>24.2494890306441</v>
+        <v>24.24948903064409</v>
       </c>
     </row>
     <row r="4984" spans="1:2">
@@ -40359,7 +40359,7 @@
         <v>5002</v>
       </c>
       <c r="B5002">
-        <v>3.256927759747397</v>
+        <v>3.256927759747396</v>
       </c>
     </row>
     <row r="5003" spans="1:2">
@@ -40367,7 +40367,7 @@
         <v>5003</v>
       </c>
       <c r="B5003">
-        <v>5.910539479306547</v>
+        <v>5.910539479306546</v>
       </c>
     </row>
     <row r="5004" spans="1:2">
@@ -40399,7 +40399,7 @@
         <v>5007</v>
       </c>
       <c r="B5007">
-        <v>8.907513227761331</v>
+        <v>8.90751322776133</v>
       </c>
     </row>
     <row r="5008" spans="1:2">
@@ -40423,7 +40423,7 @@
         <v>5010</v>
       </c>
       <c r="B5010">
-        <v>7.515337872808343</v>
+        <v>7.515337872808342</v>
       </c>
     </row>
     <row r="5011" spans="1:2">
@@ -40935,7 +40935,7 @@
         <v>5074</v>
       </c>
       <c r="B5074">
-        <v>20.80323737992148</v>
+        <v>20.80323737992147</v>
       </c>
     </row>
     <row r="5075" spans="1:2">
@@ -41031,7 +41031,7 @@
         <v>5086</v>
       </c>
       <c r="B5086">
-        <v>5.725259968664846</v>
+        <v>5.725259968664845</v>
       </c>
     </row>
     <row r="5087" spans="1:2">
@@ -41055,7 +41055,7 @@
         <v>5089</v>
       </c>
       <c r="B5089">
-        <v>4.548110834777686</v>
+        <v>4.548110834777685</v>
       </c>
     </row>
     <row r="5090" spans="1:2">
@@ -41231,7 +41231,7 @@
         <v>5111</v>
       </c>
       <c r="B5111">
-        <v>9.434425648170564</v>
+        <v>9.434425648170562</v>
       </c>
     </row>
     <row r="5112" spans="1:2">
@@ -41247,7 +41247,7 @@
         <v>5113</v>
       </c>
       <c r="B5113">
-        <v>8.63639320989572</v>
+        <v>8.636393209895719</v>
       </c>
     </row>
     <row r="5114" spans="1:2">
@@ -41367,7 +41367,7 @@
         <v>5128</v>
       </c>
       <c r="B5128">
-        <v>29.51518430358409</v>
+        <v>29.51518430358408</v>
       </c>
     </row>
     <row r="5129" spans="1:2">
@@ -41463,7 +41463,7 @@
         <v>5140</v>
       </c>
       <c r="B5140">
-        <v>8.025369401390682</v>
+        <v>8.02536940139068</v>
       </c>
     </row>
     <row r="5141" spans="1:2">
@@ -41471,7 +41471,7 @@
         <v>5141</v>
       </c>
       <c r="B5141">
-        <v>9.685851292238132</v>
+        <v>9.68585129223813</v>
       </c>
     </row>
     <row r="5142" spans="1:2">
@@ -41647,7 +41647,7 @@
         <v>5163</v>
       </c>
       <c r="B5163">
-        <v>4.584744714610354</v>
+        <v>4.584744714610353</v>
       </c>
     </row>
     <row r="5164" spans="1:2">
@@ -41671,7 +41671,7 @@
         <v>5166</v>
       </c>
       <c r="B5166">
-        <v>3.402290994923424</v>
+        <v>3.402290994923423</v>
       </c>
     </row>
     <row r="5167" spans="1:2">
@@ -41703,7 +41703,7 @@
         <v>5170</v>
       </c>
       <c r="B5170">
-        <v>12.77804382115399</v>
+        <v>12.77804382115398</v>
       </c>
     </row>
     <row r="5171" spans="1:2">
@@ -41799,7 +41799,7 @@
         <v>5182</v>
       </c>
       <c r="B5182">
-        <v>12.21259255916079</v>
+        <v>12.21259255916078</v>
       </c>
     </row>
     <row r="5183" spans="1:2">
@@ -41959,7 +41959,7 @@
         <v>5202</v>
       </c>
       <c r="B5202">
-        <v>5.325950678488763</v>
+        <v>5.325950678488762</v>
       </c>
     </row>
     <row r="5203" spans="1:2">
@@ -42103,7 +42103,7 @@
         <v>5220</v>
       </c>
       <c r="B5220">
-        <v>8.801128440727263</v>
+        <v>8.801128440727261</v>
       </c>
     </row>
     <row r="5221" spans="1:2">
@@ -42271,7 +42271,7 @@
         <v>5241</v>
       </c>
       <c r="B5241">
-        <v>4.842910992567133</v>
+        <v>4.842910992567132</v>
       </c>
     </row>
     <row r="5242" spans="1:2">
@@ -42343,7 +42343,7 @@
         <v>5250</v>
       </c>
       <c r="B5250">
-        <v>7.588048797500222</v>
+        <v>7.588048797500221</v>
       </c>
     </row>
     <row r="5251" spans="1:2">
@@ -42479,7 +42479,7 @@
         <v>5267</v>
       </c>
       <c r="B5267">
-        <v>15.20048110541707</v>
+        <v>15.20048110541706</v>
       </c>
     </row>
     <row r="5268" spans="1:2">
@@ -42751,7 +42751,7 @@
         <v>5301</v>
       </c>
       <c r="B5301">
-        <v>8.125482468197397</v>
+        <v>8.125482468197395</v>
       </c>
     </row>
     <row r="5302" spans="1:2">
@@ -42991,7 +42991,7 @@
         <v>5331</v>
       </c>
       <c r="B5331">
-        <v>1.660039353579072</v>
+        <v>1.660039353579071</v>
       </c>
     </row>
     <row r="5332" spans="1:2">
@@ -43103,7 +43103,7 @@
         <v>5345</v>
       </c>
       <c r="B5345">
-        <v>12.83340494035712</v>
+        <v>12.83340494035711</v>
       </c>
     </row>
     <row r="5346" spans="1:2">
@@ -43247,7 +43247,7 @@
         <v>5363</v>
       </c>
       <c r="B5363">
-        <v>9.52475014228599</v>
+        <v>9.524750142285988</v>
       </c>
     </row>
     <row r="5364" spans="1:2">
@@ -43271,7 +43271,7 @@
         <v>5366</v>
       </c>
       <c r="B5366">
-        <v>19.4635803550966</v>
+        <v>19.46358035509659</v>
       </c>
     </row>
     <row r="5367" spans="1:2">
@@ -43303,7 +43303,7 @@
         <v>5370</v>
       </c>
       <c r="B5370">
-        <v>13.61484955784373</v>
+        <v>13.61484955784372</v>
       </c>
     </row>
     <row r="5371" spans="1:2">
@@ -43319,7 +43319,7 @@
         <v>5372</v>
       </c>
       <c r="B5372">
-        <v>7.725264657801464</v>
+        <v>7.725264657801463</v>
       </c>
     </row>
     <row r="5373" spans="1:2">
@@ -43335,7 +43335,7 @@
         <v>5374</v>
       </c>
       <c r="B5374">
-        <v>4.738196710453434</v>
+        <v>4.738196710453433</v>
       </c>
     </row>
     <row r="5375" spans="1:2">
@@ -43503,7 +43503,7 @@
         <v>5395</v>
       </c>
       <c r="B5395">
-        <v>18.52836136362438</v>
+        <v>18.52836136362437</v>
       </c>
     </row>
     <row r="5396" spans="1:2">
@@ -43631,7 +43631,7 @@
         <v>5411</v>
       </c>
       <c r="B5411">
-        <v>30.052676588489</v>
+        <v>30.05267658848899</v>
       </c>
     </row>
     <row r="5412" spans="1:2">
@@ -43671,7 +43671,7 @@
         <v>5416</v>
       </c>
       <c r="B5416">
-        <v>36.44309058649963</v>
+        <v>36.44309058649962</v>
       </c>
     </row>
     <row r="5417" spans="1:2">
@@ -43687,7 +43687,7 @@
         <v>5418</v>
       </c>
       <c r="B5418">
-        <v>24.57907672072265</v>
+        <v>24.57907672072264</v>
       </c>
     </row>
     <row r="5419" spans="1:2">
@@ -44183,7 +44183,7 @@
         <v>5480</v>
       </c>
       <c r="B5480">
-        <v>14.06005377267418</v>
+        <v>14.06005377267417</v>
       </c>
     </row>
     <row r="5481" spans="1:2">
@@ -44319,7 +44319,7 @@
         <v>5497</v>
       </c>
       <c r="B5497">
-        <v>4.863103587130899</v>
+        <v>4.863103587130898</v>
       </c>
     </row>
     <row r="5498" spans="1:2">
@@ -44327,7 +44327,7 @@
         <v>5498</v>
       </c>
       <c r="B5498">
-        <v>4.340470003886122</v>
+        <v>4.340470003886121</v>
       </c>
     </row>
     <row r="5499" spans="1:2">
@@ -44383,7 +44383,7 @@
         <v>5505</v>
       </c>
       <c r="B5505">
-        <v>3.621830509984638</v>
+        <v>3.621830509984637</v>
       </c>
     </row>
     <row r="5506" spans="1:2">
@@ -44407,7 +44407,7 @@
         <v>5508</v>
       </c>
       <c r="B5508">
-        <v>6.178787400993278</v>
+        <v>6.178787400993277</v>
       </c>
     </row>
     <row r="5509" spans="1:2">
@@ -44607,7 +44607,7 @@
         <v>5533</v>
       </c>
       <c r="B5533">
-        <v>7.950050144454716</v>
+        <v>7.950050144454715</v>
       </c>
     </row>
     <row r="5534" spans="1:2">
@@ -44623,7 +44623,7 @@
         <v>5535</v>
       </c>
       <c r="B5535">
-        <v>8.877063146844417</v>
+        <v>8.877063146844415</v>
       </c>
     </row>
     <row r="5536" spans="1:2">
@@ -44655,7 +44655,7 @@
         <v>5539</v>
       </c>
       <c r="B5539">
-        <v>4.422266130776504</v>
+        <v>4.422266130776503</v>
       </c>
     </row>
     <row r="5540" spans="1:2">
@@ -44759,7 +44759,7 @@
         <v>5552</v>
       </c>
       <c r="B5552">
-        <v>15.00995562318333</v>
+        <v>15.00995562318332</v>
       </c>
     </row>
     <row r="5553" spans="1:2">
@@ -44895,7 +44895,7 @@
         <v>5569</v>
       </c>
       <c r="B5569">
-        <v>7.683296885065159</v>
+        <v>7.683296885065158</v>
       </c>
     </row>
     <row r="5570" spans="1:2">
@@ -44919,7 +44919,7 @@
         <v>5572</v>
       </c>
       <c r="B5572">
-        <v>5.800637839808543</v>
+        <v>5.800637839808542</v>
       </c>
     </row>
     <row r="5573" spans="1:2">
@@ -44927,7 +44927,7 @@
         <v>5573</v>
       </c>
       <c r="B5573">
-        <v>7.176958051569953</v>
+        <v>7.176958051569952</v>
       </c>
     </row>
     <row r="5574" spans="1:2">
@@ -44975,7 +44975,7 @@
         <v>5579</v>
       </c>
       <c r="B5579">
-        <v>23.78813660158341</v>
+        <v>23.7881366015834</v>
       </c>
     </row>
     <row r="5580" spans="1:2">
@@ -45079,7 +45079,7 @@
         <v>5592</v>
       </c>
       <c r="B5592">
-        <v>5.163706551485841</v>
+        <v>5.16370655148584</v>
       </c>
     </row>
     <row r="5593" spans="1:2">
@@ -45127,7 +45127,7 @@
         <v>5598</v>
       </c>
       <c r="B5598">
-        <v>9.433106828496587</v>
+        <v>9.433106828496586</v>
       </c>
     </row>
     <row r="5599" spans="1:2">
@@ -45183,7 +45183,7 @@
         <v>5605</v>
       </c>
       <c r="B5605">
-        <v>23.26969393419149</v>
+        <v>23.26969393419148</v>
       </c>
     </row>
     <row r="5606" spans="1:2">
@@ -45239,7 +45239,7 @@
         <v>5612</v>
       </c>
       <c r="B5612">
-        <v>3.61787405096271</v>
+        <v>3.617874050962709</v>
       </c>
     </row>
     <row r="5613" spans="1:2">
@@ -45335,7 +45335,7 @@
         <v>5624</v>
       </c>
       <c r="B5624">
-        <v>3.953850689684076</v>
+        <v>3.953850689684075</v>
       </c>
     </row>
     <row r="5625" spans="1:2">
@@ -45527,7 +45527,7 @@
         <v>5648</v>
       </c>
       <c r="B5648">
-        <v>3.963404805544436</v>
+        <v>3.963404805544435</v>
       </c>
     </row>
     <row r="5649" spans="1:2">
@@ -45551,7 +45551,7 @@
         <v>5651</v>
       </c>
       <c r="B5651">
-        <v>12.49707661638936</v>
+        <v>12.49707661638935</v>
       </c>
     </row>
     <row r="5652" spans="1:2">
@@ -45767,7 +45767,7 @@
         <v>5678</v>
       </c>
       <c r="B5678">
-        <v>9.385805162856649</v>
+        <v>9.385805162856643</v>
       </c>
     </row>
     <row r="5679" spans="1:2">
@@ -45799,7 +45799,7 @@
         <v>5682</v>
       </c>
       <c r="B5682">
-        <v>7.132792246043688</v>
+        <v>7.132792246043687</v>
       </c>
     </row>
     <row r="5683" spans="1:2">
@@ -45975,7 +45975,7 @@
         <v>5704</v>
       </c>
       <c r="B5704">
-        <v>18.5032451756111</v>
+        <v>18.50324517561109</v>
       </c>
     </row>
     <row r="5705" spans="1:2">
@@ -46087,7 +46087,7 @@
         <v>5718</v>
       </c>
       <c r="B5718">
-        <v>7.092934584785745</v>
+        <v>7.092934584785744</v>
       </c>
     </row>
     <row r="5719" spans="1:2">
@@ -46183,7 +46183,7 @@
         <v>5730</v>
       </c>
       <c r="B5730">
-        <v>18.2023491402175</v>
+        <v>18.20234914021749</v>
       </c>
     </row>
     <row r="5731" spans="1:2">
@@ -46207,7 +46207,7 @@
         <v>5733</v>
       </c>
       <c r="B5733">
-        <v>8.477753856668334</v>
+        <v>8.477753856668333</v>
       </c>
     </row>
     <row r="5734" spans="1:2">
@@ -46231,7 +46231,7 @@
         <v>5736</v>
       </c>
       <c r="B5736">
-        <v>6.176706596618781</v>
+        <v>6.17670659661878</v>
       </c>
     </row>
     <row r="5737" spans="1:2">
@@ -46287,7 +46287,7 @@
         <v>5743</v>
       </c>
       <c r="B5743">
-        <v>13.9909769288617</v>
+        <v>13.99097692886169</v>
       </c>
     </row>
     <row r="5744" spans="1:2">
@@ -46319,7 +46319,7 @@
         <v>5747</v>
       </c>
       <c r="B5747">
-        <v>21.21359544825509</v>
+        <v>21.21359544825508</v>
       </c>
     </row>
     <row r="5748" spans="1:2">
@@ -46327,7 +46327,7 @@
         <v>5748</v>
       </c>
       <c r="B5748">
-        <v>25.31131471081802</v>
+        <v>25.31131471081801</v>
       </c>
     </row>
     <row r="5749" spans="1:2">
@@ -46375,7 +46375,7 @@
         <v>5754</v>
       </c>
       <c r="B5754">
-        <v>17.78571935165653</v>
+        <v>17.78571935165652</v>
       </c>
     </row>
     <row r="5755" spans="1:2">
@@ -46423,7 +46423,7 @@
         <v>5760</v>
       </c>
       <c r="B5760">
-        <v>9.682598203708991</v>
+        <v>9.68259820370899</v>
       </c>
     </row>
     <row r="5761" spans="1:2">
@@ -46439,7 +46439,7 @@
         <v>5762</v>
       </c>
       <c r="B5762">
-        <v>8.431888239117834</v>
+        <v>8.431888239117832</v>
       </c>
     </row>
     <row r="5763" spans="1:2">
@@ -46599,7 +46599,7 @@
         <v>5782</v>
       </c>
       <c r="B5782">
-        <v>2.52553381424337</v>
+        <v>2.525533814243369</v>
       </c>
     </row>
     <row r="5783" spans="1:2">
@@ -46671,7 +46671,7 @@
         <v>5791</v>
       </c>
       <c r="B5791">
-        <v>2.31810692521003</v>
+        <v>2.318106925210029</v>
       </c>
     </row>
     <row r="5792" spans="1:2">
@@ -46687,7 +46687,7 @@
         <v>5793</v>
       </c>
       <c r="B5793">
-        <v>11.66027087969962</v>
+        <v>11.66027087969961</v>
       </c>
     </row>
     <row r="5794" spans="1:2">
@@ -46735,7 +46735,7 @@
         <v>5799</v>
       </c>
       <c r="B5799">
-        <v>23.98018605321819</v>
+        <v>23.98018605321818</v>
       </c>
     </row>
     <row r="5800" spans="1:2">
@@ -46751,7 +46751,7 @@
         <v>5801</v>
       </c>
       <c r="B5801">
-        <v>18.31729160158048</v>
+        <v>18.31729160158047</v>
       </c>
     </row>
     <row r="5802" spans="1:2">
@@ -46943,7 +46943,7 @@
         <v>5825</v>
       </c>
       <c r="B5825">
-        <v>21.81864060757144</v>
+        <v>21.81864060757143</v>
       </c>
     </row>
     <row r="5826" spans="1:2">
@@ -46991,7 +46991,7 @@
         <v>5831</v>
       </c>
       <c r="B5831">
-        <v>6.859298352764921</v>
+        <v>6.85929835276492</v>
       </c>
     </row>
     <row r="5832" spans="1:2">
@@ -46999,7 +46999,7 @@
         <v>5832</v>
       </c>
       <c r="B5832">
-        <v>5.396756641429343</v>
+        <v>5.396756641429342</v>
       </c>
     </row>
     <row r="5833" spans="1:2">
@@ -47103,7 +47103,7 @@
         <v>5845</v>
       </c>
       <c r="B5845">
-        <v>13.34554658041782</v>
+        <v>13.34554658041781</v>
       </c>
     </row>
     <row r="5846" spans="1:2">
@@ -47159,7 +47159,7 @@
         <v>5852</v>
       </c>
       <c r="B5852">
-        <v>7.817201042629528</v>
+        <v>7.817201042629527</v>
       </c>
     </row>
     <row r="5853" spans="1:2">
@@ -47319,7 +47319,7 @@
         <v>5872</v>
       </c>
       <c r="B5872">
-        <v>14.27719010521837</v>
+        <v>14.27719010521836</v>
       </c>
     </row>
     <row r="5873" spans="1:2">
@@ -47655,7 +47655,7 @@
         <v>5914</v>
       </c>
       <c r="B5914">
-        <v>0.7116907795748243</v>
+        <v>0.7116907795748242</v>
       </c>
     </row>
     <row r="5915" spans="1:2">
@@ -47663,7 +47663,7 @@
         <v>5915</v>
       </c>
       <c r="B5915">
-        <v>3.652192669589953</v>
+        <v>3.652192669589952</v>
       </c>
     </row>
     <row r="5916" spans="1:2">
@@ -47695,7 +47695,7 @@
         <v>5919</v>
       </c>
       <c r="B5919">
-        <v>14.21174734228529</v>
+        <v>14.21174734228528</v>
       </c>
     </row>
     <row r="5920" spans="1:2">
@@ -48319,7 +48319,7 @@
         <v>5997</v>
       </c>
       <c r="B5997">
-        <v>6.945519852339088</v>
+        <v>6.945519852339087</v>
       </c>
     </row>
     <row r="5998" spans="1:2">
@@ -48455,7 +48455,7 @@
         <v>6014</v>
       </c>
       <c r="B6014">
-        <v>6.292235200059084</v>
+        <v>6.292235200059083</v>
       </c>
     </row>
     <row r="6015" spans="1:2">
@@ -48479,7 +48479,7 @@
         <v>6017</v>
       </c>
       <c r="B6017">
-        <v>7.638398401942241</v>
+        <v>7.63839840194224</v>
       </c>
     </row>
     <row r="6018" spans="1:2">
@@ -48839,7 +48839,7 @@
         <v>6062</v>
       </c>
       <c r="B6062">
-        <v>22.77944470071879</v>
+        <v>22.77944470071878</v>
       </c>
     </row>
     <row r="6063" spans="1:2">
@@ -48871,7 +48871,7 @@
         <v>6066</v>
       </c>
       <c r="B6066">
-        <v>9.5316666187984</v>
+        <v>9.531666618798395</v>
       </c>
     </row>
     <row r="6067" spans="1:2">
@@ -49207,7 +49207,7 @@
         <v>6108</v>
       </c>
       <c r="B6108">
-        <v>19.41431511349763</v>
+        <v>19.41431511349762</v>
       </c>
     </row>
     <row r="6109" spans="1:2">
@@ -49271,7 +49271,7 @@
         <v>6116</v>
       </c>
       <c r="B6116">
-        <v>5.994475024779157</v>
+        <v>5.994475024779156</v>
       </c>
     </row>
     <row r="6117" spans="1:2">
@@ -49367,7 +49367,7 @@
         <v>6128</v>
       </c>
       <c r="B6128">
-        <v>7.529903503429811</v>
+        <v>7.52990350342981</v>
       </c>
     </row>
     <row r="6129" spans="1:2">
@@ -49375,7 +49375,7 @@
         <v>6129</v>
       </c>
       <c r="B6129">
-        <v>9.526068961959966</v>
+        <v>9.526068961959965</v>
       </c>
     </row>
     <row r="6130" spans="1:2">
@@ -49559,7 +49559,7 @@
         <v>6152</v>
       </c>
       <c r="B6152">
-        <v>7.339671092234732</v>
+        <v>7.339671092234731</v>
       </c>
     </row>
     <row r="6153" spans="1:2">
@@ -49615,7 +49615,7 @@
         <v>6159</v>
       </c>
       <c r="B6159">
-        <v>20.3613448678279</v>
+        <v>20.36134486782789</v>
       </c>
     </row>
     <row r="6160" spans="1:2">
@@ -49655,7 +49655,7 @@
         <v>6164</v>
       </c>
       <c r="B6164">
-        <v>3.105527261174946</v>
+        <v>3.105527261174945</v>
       </c>
     </row>
     <row r="6165" spans="1:2">
@@ -49783,7 +49783,7 @@
         <v>6180</v>
       </c>
       <c r="B6180">
-        <v>2.922413545508951</v>
+        <v>2.92241354550895</v>
       </c>
     </row>
     <row r="6181" spans="1:2">
@@ -50223,7 +50223,7 @@
         <v>6235</v>
       </c>
       <c r="B6235">
-        <v>6.794676188740095</v>
+        <v>6.794676188740094</v>
       </c>
     </row>
     <row r="6236" spans="1:2">
@@ -50351,7 +50351,7 @@
         <v>6251</v>
       </c>
       <c r="B6251">
-        <v>18.44844089138143</v>
+        <v>18.44844089138142</v>
       </c>
     </row>
     <row r="6252" spans="1:2">
@@ -50407,7 +50407,7 @@
         <v>6258</v>
       </c>
       <c r="B6258">
-        <v>11.07480286576585</v>
+        <v>11.07480286576584</v>
       </c>
     </row>
     <row r="6259" spans="1:2">
@@ -50415,7 +50415,7 @@
         <v>6259</v>
       </c>
       <c r="B6259">
-        <v>3.501964455172148</v>
+        <v>3.501964455172147</v>
       </c>
     </row>
     <row r="6260" spans="1:2">
@@ -50575,7 +50575,7 @@
         <v>6279</v>
       </c>
       <c r="B6279">
-        <v>27.6439257217314</v>
+        <v>27.64392572173139</v>
       </c>
     </row>
     <row r="6280" spans="1:2">
@@ -50631,7 +50631,7 @@
         <v>6286</v>
       </c>
       <c r="B6286">
-        <v>3.852741181345912</v>
+        <v>3.852741181345911</v>
       </c>
     </row>
     <row r="6287" spans="1:2">
@@ -50655,7 +50655,7 @@
         <v>6289</v>
       </c>
       <c r="B6289">
-        <v>3.257455287616987</v>
+        <v>3.257455287616986</v>
       </c>
     </row>
     <row r="6290" spans="1:2">
@@ -50711,7 +50711,7 @@
         <v>6296</v>
       </c>
       <c r="B6296">
-        <v>16.7997990704959</v>
+        <v>16.79979907049589</v>
       </c>
     </row>
     <row r="6297" spans="1:2">
@@ -50743,7 +50743,7 @@
         <v>6300</v>
       </c>
       <c r="B6300">
-        <v>24.26806973449523</v>
+        <v>24.26806973449522</v>
       </c>
     </row>
     <row r="6301" spans="1:2">
@@ -50911,7 +50911,7 @@
         <v>6321</v>
       </c>
       <c r="B6321">
-        <v>3.702425045616508</v>
+        <v>3.702425045616507</v>
       </c>
     </row>
     <row r="6322" spans="1:2">
@@ -50959,7 +50959,7 @@
         <v>6327</v>
       </c>
       <c r="B6327">
-        <v>14.45514283989354</v>
+        <v>14.45514283989353</v>
       </c>
     </row>
     <row r="6328" spans="1:2">
@@ -50975,7 +50975,7 @@
         <v>6329</v>
       </c>
       <c r="B6329">
-        <v>6.178523637058482</v>
+        <v>6.178523637058481</v>
       </c>
     </row>
     <row r="6330" spans="1:2">
@@ -52295,7 +52295,7 @@
         <v>6494</v>
       </c>
       <c r="B6494">
-        <v>4.89554655111071</v>
+        <v>4.895546551110709</v>
       </c>
     </row>
     <row r="6495" spans="1:2">
@@ -53087,7 +53087,7 @@
         <v>6593</v>
       </c>
       <c r="B6593">
-        <v>7.430464500012016</v>
+        <v>7.430464500012015</v>
       </c>
     </row>
     <row r="6594" spans="1:2">
@@ -53607,7 +53607,7 @@
         <v>6658</v>
       </c>
       <c r="B6658">
-        <v>7.03868713552953</v>
+        <v>7.038687135529529</v>
       </c>
     </row>
     <row r="6659" spans="1:2">
@@ -54799,7 +54799,7 @@
         <v>6807</v>
       </c>
       <c r="B6807">
-        <v>7.469179184219181</v>
+        <v>7.46917918421918</v>
       </c>
     </row>
     <row r="6808" spans="1:2">
@@ -55007,7 +55007,7 @@
         <v>6833</v>
       </c>
       <c r="B6833">
-        <v>5.897116825735858</v>
+        <v>5.897116825735857</v>
       </c>
     </row>
     <row r="6834" spans="1:2">
@@ -55559,7 +55559,7 @@
         <v>6902</v>
       </c>
       <c r="B6902">
-        <v>6.288718347595148</v>
+        <v>6.288718347595147</v>
       </c>
     </row>
     <row r="6903" spans="1:2">
@@ -55759,7 +55759,7 @@
         <v>6927</v>
       </c>
       <c r="B6927">
-        <v>8.712620987051537</v>
+        <v>8.712620987051535</v>
       </c>
     </row>
     <row r="6928" spans="1:2">
@@ -57119,7 +57119,7 @@
         <v>7097</v>
       </c>
       <c r="B7097">
-        <v>6.803058020445809</v>
+        <v>6.803058020445808</v>
       </c>
     </row>
     <row r="7098" spans="1:2">
@@ -57303,7 +57303,7 @@
         <v>7120</v>
       </c>
       <c r="B7120">
-        <v>17.3540843259161</v>
+        <v>17.35408432591609</v>
       </c>
     </row>
     <row r="7121" spans="1:2">
@@ -57511,7 +57511,7 @@
         <v>7146</v>
       </c>
       <c r="B7146">
-        <v>2.443245328008038</v>
+        <v>2.443245328008037</v>
       </c>
     </row>
     <row r="7147" spans="1:2">

</xml_diff>